<commit_message>
add data for budget specific parameters
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaep/code/sti/sti_budget_simulator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F71607-5F3C-2C4B-A4F3-39EB4680D80A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DD5271-5D16-AC4D-8912-3EFB1090B9B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="66660" yWindow="9400" windowWidth="27640" windowHeight="16940" xr2:uid="{9DEAE40D-0FFE-824B-8508-973FB79CDC2F}"/>
+    <workbookView xWindow="32380" yWindow="5860" windowWidth="18820" windowHeight="17540" xr2:uid="{9DEAE40D-0FFE-824B-8508-973FB79CDC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,14 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>CF</t>
   </si>
   <si>
-    <t>initial budget</t>
-  </si>
-  <si>
     <t>academic rank</t>
   </si>
   <si>
@@ -51,6 +48,18 @@
   </si>
   <si>
     <t>PATT</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>PATT yearly budget</t>
+  </si>
+  <si>
+    <t>PA yearly budget</t>
+  </si>
+  <si>
+    <t>PO yearly budget</t>
   </si>
 </sst>
 </file>
@@ -403,7 +412,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D4BE15F-799F-2F47-B7E3-65508FA76526}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
@@ -412,12 +421,15 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -428,35 +440,50 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1234</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1">
         <v>43101</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>4567</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>36526</v>
       </c>
       <c r="D3" s="1">
-        <v>36526</v>
+        <v>21916</v>
+      </c>
+      <c r="E3">
+        <v>12000</v>
+      </c>
+      <c r="F3">
+        <v>120000</v>
+      </c>
+      <c r="G3">
+        <v>240000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>